<commit_message>
Updated code with extent reports setup
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialsNinja/testData/TutorialsNinjaTestData.xlsx
+++ b/src/main/java/com/tutorialsNinja/testData/TutorialsNinjaTestData.xlsx
@@ -41,7 +41,7 @@
     <t>aftabalimulla32@gmail.com</t>
   </si>
   <si>
-    <t>aftabalimulla34@gmail.com</t>
+    <t>aftabalimulla33@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>